<commit_message>
Update summary result on clustering.xlsx
</commit_message>
<xml_diff>
--- a/summary result on clustering.xlsx
+++ b/summary result on clustering.xlsx
@@ -274,6 +274,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -413,12 +419,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +607,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -631,16 +631,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -649,67 +649,67 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -731,7 +731,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -741,12 +741,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1069,7 +1066,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1118,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="3">
-        <v>0.096</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1157,7 +1154,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="3">
-        <v>0.002</v>
+        <v>0.05</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -1261,7 +1258,7 @@
       <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="9">
         <v>0.52</v>
       </c>
     </row>
@@ -1331,28 +1328,28 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="3">
         <v>0.096</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="3">
         <v>0.094</v>
       </c>
     </row>
@@ -1373,12 +1370,12 @@
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="11">
         <v>0.61</v>
       </c>
     </row>

</xml_diff>